<commit_message>
Apply rounding function for coefficients (xls)
</commit_message>
<xml_diff>
--- a/Source Code/Coeff_gen/coefficients_source.xlsx
+++ b/Source Code/Coeff_gen/coefficients_source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GDRIVE\Jericho-Lab\5_IT\Jericho-github-repo\rdl\Source Code\Coeff_gen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GDRIVE\Jericho-Lab\7_Engineering_R-D\1-RDL\RDL-Experiments\2025-04-09-Strain-Hysteresis-48h-WIP\Coeff_gen_both\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026DC27F-1E09-47C3-8B1B-F72610EF407F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0F97C6-E9F3-48EB-BDDD-437ABB1A15EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,6 +139,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,9 +306,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,6 +313,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -482,13 +485,13 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>549</c:v>
+                  <c:v>23713</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14078.391777098199</c:v>
+                  <c:v>65183.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>135842.91777098199</c:v>
+                  <c:v>438418</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,13 +578,13 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>555</c:v>
+                  <c:v>-171611</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51460.538566089017</c:v>
+                  <c:v>-130495.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>509610.38566089014</c:v>
+                  <c:v>239548</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -668,13 +671,13 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>549</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68444.684675501194</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>679505.84675501194</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2170,7 +2173,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2195,11 +2198,11 @@
       <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="M4" s="4" t="s">
         <v>26</v>
       </c>
@@ -2211,11 +2214,11 @@
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="M5" t="s">
         <v>14</v>
       </c>
@@ -2247,25 +2250,25 @@
       <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="C7" s="14">
-        <f t="shared" ref="C7:C14" si="0">(E34-D34)/(9.81*$E$30)</f>
-        <v>1352.9391777098199</v>
+      <c r="C7" s="17">
+        <f>ROUND((E34-D34)/(9.81*$E$30),2)</f>
+        <v>4147.05</v>
       </c>
       <c r="D7" s="7">
         <f>D34</f>
-        <v>549</v>
-      </c>
-      <c r="F7" s="15">
+        <v>23713</v>
+      </c>
+      <c r="F7" s="14">
         <f>D7</f>
-        <v>549</v>
-      </c>
-      <c r="G7" s="15">
+        <v>23713</v>
+      </c>
+      <c r="G7" s="14">
         <f>D7+C7*10</f>
-        <v>14078.391777098199</v>
-      </c>
-      <c r="H7" s="15">
+        <v>65183.5</v>
+      </c>
+      <c r="H7" s="14">
         <f>D7+C7*100</f>
-        <v>135842.91777098199</v>
+        <v>438418</v>
       </c>
       <c r="M7" t="s">
         <v>0</v>
@@ -2275,25 +2278,25 @@
       <c r="B8" s="5">
         <v>2</v>
       </c>
-      <c r="C8" s="14">
-        <f t="shared" si="0"/>
-        <v>5090.5538566089017</v>
+      <c r="C8" s="17">
+        <f t="shared" ref="C8:C14" si="0">ROUND((E35-D35)/(9.81*$E$30),2)</f>
+        <v>4111.59</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" ref="D8:D14" si="1">D35</f>
-        <v>555</v>
-      </c>
-      <c r="F8" s="15">
+        <v>-171611</v>
+      </c>
+      <c r="F8" s="14">
         <f t="shared" ref="F8:F14" si="2">D8</f>
-        <v>555</v>
-      </c>
-      <c r="G8" s="15">
+        <v>-171611</v>
+      </c>
+      <c r="G8" s="14">
         <f t="shared" ref="G8:G14" si="3">D8+C8*10</f>
-        <v>51460.538566089017</v>
-      </c>
-      <c r="H8" s="15">
+        <v>-130495.1</v>
+      </c>
+      <c r="H8" s="14">
         <f t="shared" ref="H8:H14" si="4">D8+C8*100</f>
-        <v>509610.38566089014</v>
+        <v>239548</v>
       </c>
       <c r="M8" t="s">
         <v>1</v>
@@ -2303,25 +2306,25 @@
       <c r="B9" s="5">
         <v>3</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="17">
         <f t="shared" si="0"/>
-        <v>6789.5684675501188</v>
+        <v>0</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" si="1"/>
-        <v>549</v>
-      </c>
-      <c r="F9" s="15">
+        <v>0</v>
+      </c>
+      <c r="F9" s="14">
         <f t="shared" si="2"/>
-        <v>549</v>
-      </c>
-      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
         <f t="shared" si="3"/>
-        <v>68444.684675501194</v>
-      </c>
-      <c r="H9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14">
         <f t="shared" si="4"/>
-        <v>679505.84675501194</v>
+        <v>0</v>
       </c>
       <c r="M9" t="s">
         <v>7</v>
@@ -2331,7 +2334,7 @@
       <c r="B10" s="5">
         <v>4</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2339,15 +2342,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2359,7 +2362,7 @@
       <c r="B11" s="5">
         <v>5</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2367,15 +2370,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2387,7 +2390,7 @@
       <c r="B12" s="5">
         <v>6</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2395,15 +2398,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2412,7 +2415,7 @@
       <c r="B13" s="5">
         <v>7</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2420,15 +2423,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2437,7 +2440,7 @@
       <c r="B14" s="5">
         <v>8</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2445,15 +2448,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2533,7 +2536,7 @@
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="2">
-        <v>9</v>
+        <v>1.2190000000000001</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>13</v>
@@ -2566,10 +2569,10 @@
         <v>1011</v>
       </c>
       <c r="D34" s="1">
-        <v>549</v>
+        <v>23713</v>
       </c>
       <c r="E34" s="1">
-        <v>120000</v>
+        <v>73305</v>
       </c>
       <c r="F34" t="s">
         <v>32</v>
@@ -2583,10 +2586,10 @@
         <v>1012</v>
       </c>
       <c r="D35" s="1">
-        <v>555</v>
+        <v>-171611</v>
       </c>
       <c r="E35" s="1">
-        <v>450000</v>
+        <v>-122443</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -2597,10 +2600,10 @@
         <v>1013</v>
       </c>
       <c r="D36" s="1">
-        <v>549</v>
+        <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>600000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>